<commit_message>
Avance Oct 1 2019
</commit_message>
<xml_diff>
--- a/Articulo Estado Arte/Lecturas.xlsx
+++ b/Articulo Estado Arte/Lecturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sin definir\Desktop\ModelosED\ModelosED\Articulo Estado Arte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F54236A-A1E3-4096-95CD-3893BFC32961}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD65D8AC-79F2-468B-999B-6610A4C9095F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8685" xr2:uid="{12022957-D163-4B94-ACE8-46A017715E34}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve"> Tawfik. A, Rakha. H, Member and  Miller.S (2010) "Driver Route Choice Behavior: Experiences, Perceptions, and Choices"</t>
   </si>
@@ -59,6 +59,12 @@
   <si>
     <t>[1] Jan O, Horowitz A, Peng Z-R (2000) Using global positioning system data to understand variations in path choice. Transp Res Rec 1725:37–44.
 [2] Parkany E, Du J, Aultman-Hall L, Gallagher R (2006) Modeling stated and revealed route choice: consideration of consistency, diversion, and attitudinal variables. Transp Res Rec 1985:29–39</t>
+  </si>
+  <si>
+    <t>Desde la perspectiva de la toma de decisiones, la investigación de elección de ruta se enfrenta a una serie de desafíos. El primero es comprender los patrones de comportamiento subyacentes exhibidos en las preferencias individuales. Los modeladores de transporte deben tomar nota de cómo se toman las decisiones de elección de ruta. Para algunas personas, reducir la distancia es un objetivo principal, mientras que para otras, es importante minimizar el tiempo de viaje o la cantidad de giros a la izquierda. Para otros, las preferencias personales como el hábito o el conocimiento de la ruta local son el factor determinante.</t>
+  </si>
+  <si>
+    <t>Papinski, D. Scott, D. Doherty, S. (2009) Exploring the route choice decision-making process: A comparison of planned and observed routes obtained using person-based GPS</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -118,6 +124,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EAA10F-DA56-474A-9886-CB7A74CB587B}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +486,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>